<commit_message>
pdf latest everything up to date
</commit_message>
<xml_diff>
--- a/database1.xlsx
+++ b/database1.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rishu jain\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rishu jain\OneDrive\Desktop\mahesh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75FFD72C-D560-45D3-BA9B-D5BBEC19AC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4430CA9-61D0-44EA-B464-B172DE1233B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{820CAFDE-5007-44A0-BAAD-6F8296BF7F6D}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{820CAFDE-5007-44A0-BAAD-6F8296BF7F6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="accounts_rows" sheetId="1" r:id="rId1"/>
+    <sheet name="ts" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="101">
   <si>
     <t>id</t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>Mr. R Srinivasa Reddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">office type </t>
+  </si>
+  <si>
+    <t>Headquarter</t>
   </si>
 </sst>
 </file>
@@ -833,7 +839,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -855,9 +861,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -917,6 +920,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1236,25 +1243,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6658C8D1-F279-44D5-B60F-D7FDBAF3E9E8}">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.88671875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="36.5546875" style="2" customWidth="1"/>
-    <col min="3" max="7" width="27.88671875" style="2"/>
-    <col min="8" max="8" width="31.44140625" style="7" customWidth="1"/>
-    <col min="9" max="13" width="27.88671875" style="2"/>
-    <col min="14" max="14" width="33" style="2" customWidth="1"/>
-    <col min="15" max="15" width="34" style="2" customWidth="1"/>
-    <col min="17" max="17" width="63.88671875" customWidth="1"/>
+    <col min="3" max="8" width="27.88671875" style="2"/>
+    <col min="9" max="9" width="31.44140625" style="7" customWidth="1"/>
+    <col min="10" max="14" width="27.88671875" style="2"/>
+    <col min="15" max="15" width="33" style="2" customWidth="1"/>
+    <col min="16" max="16" width="34" style="2" customWidth="1"/>
+    <col min="18" max="18" width="63.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1277,31 +1284,34 @@
         <v>21</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1323,32 +1333,35 @@
       <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>122001</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>9466555566</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1370,107 +1383,110 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>500037</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>9790245217</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="2"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="3"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="3"/>
-      <c r="L4" s="4" t="s">
+      <c r="I4" s="3"/>
+      <c r="M4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>9491114007</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="4"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="3"/>
-      <c r="L5" s="2" t="s">
+      <c r="I5" s="3"/>
+      <c r="M5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>9701611135</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="2"/>
+      <c r="Q5" s="4"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="3"/>
-      <c r="L6" s="4" t="s">
+      <c r="I6" s="3"/>
+      <c r="M6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="M6" s="5">
+      <c r="N6" s="5">
         <v>9908732282</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="2"/>
+      <c r="Q6" s="4"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1492,23 +1508,26 @@
       <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>500082</v>
       </c>
-      <c r="S7" s="4"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="6"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="6"/>
     </row>
-    <row r="8" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1530,32 +1549,35 @@
       <c r="G8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>530003</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <v>9951770327</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -1577,44 +1599,50 @@
       <c r="G9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>520010</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>9154936936</v>
       </c>
-      <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="3"/>
-      <c r="L10" s="2" t="s">
+      <c r="H10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="M10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>9550948584</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>6</v>
       </c>
@@ -1636,29 +1664,32 @@
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>500017</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>8019325308</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>7</v>
       </c>
@@ -1680,32 +1711,35 @@
       <c r="G12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>462016</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>9366517232</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="P12" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>8</v>
       </c>
@@ -1727,32 +1761,35 @@
       <c r="G13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>500073</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>9652900422</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>9</v>
       </c>
@@ -1774,30 +1811,33 @@
       <c r="G14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>302001</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <v>7986080765</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="4"/>
+      <c r="P14" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>10</v>
       </c>
@@ -1819,32 +1859,35 @@
       <c r="G15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>380015</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <v>963860002</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -1866,32 +1909,35 @@
       <c r="G16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>560038</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <v>9980700006</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>12</v>
       </c>
@@ -1907,38 +1953,41 @@
       <c r="E17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>122015</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M17" s="2">
+      <c r="N17" s="2">
         <v>9871220084</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>13</v>
       </c>
@@ -1954,39 +2003,42 @@
       <c r="E18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>505082</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="M18" s="2">
+      <c r="N18" s="2">
         <v>9866633066</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="P18" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L25" s="4"/>
+    <row r="25" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>